<commit_message>
add notebook for computational journalism presentation
</commit_message>
<xml_diff>
--- a/cleaned_data/headlines.xlsx
+++ b/cleaned_data/headlines.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="4720" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="headlines" localSheetId="0">Sheet1!$A$1:$B$138</definedName>
+    <definedName name="headlines" localSheetId="0">Sheet1!$A$1:$C$137</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -775,16 +775,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B137"/>
+  <dimension ref="A1:C137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="80.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1427,7 +1426,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>82</v>
       </c>
@@ -1435,7 +1434,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>83</v>
       </c>
@@ -1443,7 +1442,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>84</v>
       </c>
@@ -1451,7 +1450,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>85</v>
       </c>
@@ -1459,7 +1458,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>86</v>
       </c>
@@ -1467,7 +1466,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>87</v>
       </c>
@@ -1475,7 +1474,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>88</v>
       </c>
@@ -1483,7 +1482,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>89</v>
       </c>
@@ -1491,7 +1490,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>90</v>
       </c>
@@ -1499,7 +1498,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>91</v>
       </c>
@@ -1507,7 +1506,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>92</v>
       </c>
@@ -1515,15 +1514,15 @@
         <v>75</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>93</v>
       </c>
-      <c r="B92" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C92" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>94</v>
       </c>
@@ -1531,7 +1530,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>95</v>
       </c>
@@ -1539,7 +1538,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>96</v>
       </c>
@@ -1547,7 +1546,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>97</v>
       </c>

</xml_diff>